<commit_message>
Add a declaration of namespace for optional dyDescent attribute to all sheet parts (used routinely by Excel). Without a preemptive declaration, it would be written only when it was requires at each row or we would have to check all rows beforehand. First one has problem with XML parsers and second is bad from performance point of view.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
@@ -395,7 +395,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -461,7 +461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -527,7 +527,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -592,7 +592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>

</xml_diff>

<commit_message>
Update test files after decoupling of sheetId and RelId. In every case, sheetId has changed and in few the calcChain i attribute (sheetId link) has also been updated.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
@@ -6,10 +6,10 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Single Column Numbers" sheetId="2" r:id="rId2"/>
-    <x:sheet name="Single Column Strings" sheetId="3" r:id="rId3"/>
-    <x:sheet name="Single Column Mixed" sheetId="4" r:id="rId4"/>
-    <x:sheet name="Multi Column" sheetId="5" r:id="rId5"/>
+    <x:sheet name="Single Column Numbers" sheetId="1" r:id="rId2"/>
+    <x:sheet name="Single Column Strings" sheetId="2" r:id="rId3"/>
+    <x:sheet name="Single Column Mixed" sheetId="3" r:id="rId4"/>
+    <x:sheet name="Multi Column" sheetId="4" r:id="rId5"/>
   </x:sheets>
   <x:definedNames>
     <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Single Column Numbers'!$A$1:$A$7</x:definedName>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
     <x:t>Numbers</x:t>
   </x:si>

</xml_diff>